<commit_message>
Formato de cronograma e Hito 1
</commit_message>
<xml_diff>
--- a/03 Linea Base/Cronograma del Proyecto.xlsx
+++ b/03 Linea Base/Cronograma del Proyecto.xlsx
@@ -2,14 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8532"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,9 +23,171 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+  <si>
+    <t>CRONOGRAMA DEL PROYECTO</t>
+  </si>
+  <si>
+    <t>Información del proyecto</t>
+  </si>
+  <si>
+    <t>N° de grupo:</t>
+  </si>
+  <si>
+    <t>Nombre de proyecto:</t>
+  </si>
+  <si>
+    <t>Herramienta para la predicción del nivel de presión sonora escalado en decibelios</t>
+  </si>
+  <si>
+    <t>Enfoque de desarrollo:</t>
+  </si>
+  <si>
+    <t>Scrum</t>
+  </si>
+  <si>
+    <t>Inicio:</t>
+  </si>
+  <si>
+    <t>Fin:</t>
+  </si>
+  <si>
+    <t>Actividad</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Nomenclatura</t>
+  </si>
+  <si>
+    <t>Fecha Inicio</t>
+  </si>
+  <si>
+    <t>Fecha Fin</t>
+  </si>
+  <si>
+    <t>% de Avance</t>
+  </si>
+  <si>
+    <t>Reunión con el Stakeholder</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Todo el equipo</t>
+  </si>
+  <si>
+    <t>Idear Proyecto innovador</t>
+  </si>
+  <si>
+    <t>Elaborar Cronograma del Proyecto</t>
+  </si>
+  <si>
+    <t>Cronograma del Proyecto</t>
+  </si>
+  <si>
+    <t>SS-CP.XLS</t>
+  </si>
+  <si>
+    <t>Azucena, Estrada, Delgado</t>
+  </si>
+  <si>
+    <t>Desarrollar del Plan de Proyecto</t>
+  </si>
+  <si>
+    <t>Plan de Proyecto (PROJECT CHARTER)</t>
+  </si>
+  <si>
+    <t>SS-PC.DOCX</t>
+  </si>
+  <si>
+    <t>Agüero, Ocaña, Popi, Abad</t>
+  </si>
+  <si>
+    <t>Crear repositorio del proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repositorio GitHub
+</t>
+  </si>
+  <si>
+    <t>Agüero</t>
+  </si>
+  <si>
+    <t>Especificar Requisitos del Software</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requisitos</t>
+  </si>
+  <si>
+    <t>SS-DER.DOCX</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de UI</t>
+  </si>
+  <si>
+    <t>SS-DEUI.PDF</t>
+  </si>
+  <si>
+    <t>Establecer estilos para la muestra de datos</t>
+  </si>
+  <si>
+    <t>Documento de Guía de Estilos</t>
+  </si>
+  <si>
+    <t>SS-DGE.PDF</t>
+  </si>
+  <si>
+    <t>Especificar el diseño de la Base de Datos</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de la BD</t>
+  </si>
+  <si>
+    <t>SS-DEBD.DOCX</t>
+  </si>
+  <si>
+    <t>Especificar la Arquitectura y Diseño del Software</t>
+  </si>
+  <si>
+    <t>Documento de Arquitectura del Software</t>
+  </si>
+  <si>
+    <t>SS-DAS.DOCX</t>
+  </si>
+  <si>
+    <t>Reportar estado actual de los estilos y requisitos</t>
+  </si>
+  <si>
+    <t>Reporte del diseño del Desarrollo del Software</t>
+  </si>
+  <si>
+    <t>SS-RDS.DOCX</t>
+  </si>
+  <si>
+    <t>Realizar Sprint Retrospective</t>
+  </si>
+  <si>
+    <t>Reporte del Primer Sprint</t>
+  </si>
+  <si>
+    <t>SS-RPS.DOCX</t>
+  </si>
+  <si>
+    <t>Hito 1 - Fin del Sprint #1</t>
+  </si>
+  <si>
+    <t>Encargado(s)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +195,89 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF0779E4"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0779E4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -45,12 +285,233 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +792,455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.45" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="44.77734375" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" customWidth="1"/>
+    <col min="6" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="23">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="24">
+        <v>44818</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="24">
+        <v>44890</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="4">
+        <v>44818</v>
+      </c>
+      <c r="G11" s="4">
+        <v>44825</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="4">
+        <v>44818</v>
+      </c>
+      <c r="G12" s="4">
+        <v>44825</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="4">
+        <v>44818</v>
+      </c>
+      <c r="G13" s="4">
+        <v>44825</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="4">
+        <v>44818</v>
+      </c>
+      <c r="G14" s="4">
+        <v>44825</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="4">
+        <v>44818</v>
+      </c>
+      <c r="G15" s="4">
+        <v>44825</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="4">
+        <v>44825</v>
+      </c>
+      <c r="G16" s="4">
+        <v>44832</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="4">
+        <v>44825</v>
+      </c>
+      <c r="G17" s="4">
+        <v>44832</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="4">
+        <v>44825</v>
+      </c>
+      <c r="G18" s="4">
+        <v>44832</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
+      <c r="B19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="4">
+        <v>44839</v>
+      </c>
+      <c r="G19" s="4">
+        <v>44846</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+      <c r="B20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="4">
+        <v>44839</v>
+      </c>
+      <c r="G20" s="4">
+        <v>44846</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="4">
+        <v>44839</v>
+      </c>
+      <c r="G21" s="4">
+        <v>44846</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="4">
+        <v>44839</v>
+      </c>
+      <c r="G22" s="4">
+        <v>44846</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="21">
+        <f>AVERAGE(H11:H22)</f>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>